<commit_message>
Add support for data
But there is a big problema, data is not referenced to main process so it only creates a copy.

Next step, create a syncronous version without concurrency to get something working.
</commit_message>
<xml_diff>
--- a/data/simulator_config.xlsx
+++ b/data/simulator_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel\git\lab-events-simulator\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AngelFernandez\git\lab-events-simulator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{494B04FC-DAC6-43F2-A934-C5F18B958691}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A77F620-B61D-46C3-A306-45171D815CB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{A49770C9-701F-43A8-9FA9-C3FBCD6AD4BA}"/>
   </bookViews>
@@ -705,7 +705,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +831,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>8</v>

</xml_diff>